<commit_message>
updated cv_burial.xlsx and added missing autocompletes
</commit_message>
<xml_diff>
--- a/data/skos/cv_burial.xlsx
+++ b/data/skos/cv_burial.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="244">
   <si>
     <t xml:space="preserve">conceptScheme</t>
   </si>
@@ -713,6 +713,45 @@
   </si>
   <si>
     <t xml:space="preserve">V (more than 800°C)|V (ab 800°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burial Filling Objects| Grabfüllungsobjekte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pebble stone|Kieselstein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bigger stone|größere Steine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ceramic sherd|Scherbenschüttung (Keramikbruchstücke?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">secondary cremated ceramic sherds|Scherben - sekundär gebrannt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">human remains|Menschenknochen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">animal remains|Tierknochen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snail/shell|Schnecke/Muschel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burial Filling Type|Art der Grabfüllung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monophase and unburnt|einphasig – ungebrannt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monophase and burnt|einphasig – gebrannt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multi phase and unburnt|mehrphasig – ungebrannt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multi phase and burnt|mehrphasig – gebrannt</t>
   </si>
 </sst>
 </file>
@@ -788,12 +827,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -814,17 +861,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D206"/>
+  <dimension ref="A1:D217"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B97" activeCellId="0" sqref="B97:B98"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B217" activeCellId="0" sqref="B217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="60.6122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="70.3826530612245"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="61.6632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="71.4897959183674"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="34.4489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2708,6 +2755,94 @@
       </c>
       <c r="B206" s="1" t="s">
         <v>230</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed cv_burial.xlsx (according to https://redmine.acdh.oeaw.ac.at/issues/7585?issue_count=20&issue_position=16&next_issue_id=7577&prev_issue_id=7587#note-3) and adapted forms accordingly
</commit_message>
<xml_diff>
--- a/data/skos/cv_burial.xlsx
+++ b/data/skos/cv_burial.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="245">
   <si>
     <t xml:space="preserve">conceptScheme</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t xml:space="preserve">in the pit filling|in der Grabverfüllung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GraveGoodObject</t>
   </si>
   <si>
     <t xml:space="preserve">Accessory vessels|Beigefäße</t>
@@ -827,16 +830,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -863,15 +862,15 @@
   </sheetPr>
   <dimension ref="A1:D217"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A190" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B217" activeCellId="0" sqref="B217"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A136" activeCellId="0" sqref="A136:A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="61.6632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="71.4897959183674"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="34.4489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="62.7448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="72.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="34.9897959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2189,660 +2188,807 @@
         <v>157</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="s">
+    <row r="136" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="s">
+    <row r="137" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="138" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="s">
+      <c r="C137" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B138" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C138" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="s">
+    <row r="139" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="s">
+    <row r="142" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C147" s="1" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="149" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="1" t="s">
+      <c r="C148" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B159" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="s">
-        <v>180</v>
+    </row>
+    <row r="160" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="161" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="s">
-        <v>180</v>
+      <c r="C160" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C166" s="1" t="s">
         <v>188</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="168" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="s">
-        <v>188</v>
+      <c r="C167" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C176" s="1" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="178" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="s">
-        <v>199</v>
+      <c r="C177" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>158</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>167</v>
+        <v>200</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B214" s="3" t="s">
         <v>240</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B215" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B216" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
* updated skos vocabs * improved detail view template for burial_detail.html * implemented hopefully more meaning full self-representation strings
</commit_message>
<xml_diff>
--- a/data/skos/cv_burial.xlsx
+++ b/data/skos/cv_burial.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="253">
   <si>
     <t xml:space="preserve">conceptScheme</t>
   </si>
@@ -755,6 +755,30 @@
   </si>
   <si>
     <t xml:space="preserve">multi phase and burnt|mehrphasig – gebrannt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species | Tierart </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cattle|Rind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pig|Schwein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheep|Schaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goat|Ziege</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheep/goat|Schaf/Ziege</t>
+  </si>
+  <si>
+    <t xml:space="preserve">game meat|Wild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fish|Fisch</t>
   </si>
 </sst>
 </file>
@@ -764,7 +788,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -786,6 +810,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -830,7 +859,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -840,6 +869,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -860,17 +893,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D217"/>
+  <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A148" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A136" activeCellId="0" sqref="A136:A184"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A196" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B226" activeCellId="0" sqref="B226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="62.7448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="72.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="34.9897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="63.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="73.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="35.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1979,6 +2012,7 @@
       <c r="B109" s="1" t="s">
         <v>128</v>
       </c>
+      <c r="C109" s="0"/>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1" t="s">
@@ -1987,6 +2021,7 @@
       <c r="B110" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="C110" s="0"/>
     </row>
     <row r="111" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
@@ -1995,6 +2030,7 @@
       <c r="B111" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="C111" s="0"/>
     </row>
     <row r="112" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="1" t="s">
@@ -2003,6 +2039,7 @@
       <c r="B112" s="1" t="s">
         <v>132</v>
       </c>
+      <c r="C112" s="0"/>
     </row>
     <row r="113" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
@@ -2011,6 +2048,7 @@
       <c r="B113" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="C113" s="0"/>
     </row>
     <row r="114" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="1" t="s">
@@ -2019,6 +2057,7 @@
       <c r="B114" s="1" t="s">
         <v>134</v>
       </c>
+      <c r="C114" s="0"/>
     </row>
     <row r="115" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1" t="s">
@@ -2027,6 +2066,7 @@
       <c r="B115" s="1" t="s">
         <v>135</v>
       </c>
+      <c r="C115" s="0"/>
     </row>
     <row r="116" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1" t="s">
@@ -2035,6 +2075,7 @@
       <c r="B116" s="1" t="s">
         <v>136</v>
       </c>
+      <c r="C116" s="0"/>
     </row>
     <row r="117" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="1" t="s">
@@ -2043,6 +2084,7 @@
       <c r="B117" s="1" t="s">
         <v>137</v>
       </c>
+      <c r="C117" s="0"/>
     </row>
     <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
@@ -2051,6 +2093,7 @@
       <c r="B118" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="C118" s="0"/>
     </row>
     <row r="119" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1" t="s">
@@ -2059,6 +2102,7 @@
       <c r="B119" s="1" t="s">
         <v>140</v>
       </c>
+      <c r="C119" s="0"/>
     </row>
     <row r="120" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
@@ -2067,6 +2111,7 @@
       <c r="B120" s="1" t="s">
         <v>141</v>
       </c>
+      <c r="C120" s="0"/>
     </row>
     <row r="121" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
@@ -2075,6 +2120,7 @@
       <c r="B121" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="C121" s="0"/>
     </row>
     <row r="122" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1" t="s">
@@ -2083,6 +2129,7 @@
       <c r="B122" s="1" t="s">
         <v>143</v>
       </c>
+      <c r="C122" s="0"/>
     </row>
     <row r="123" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
@@ -2091,6 +2138,7 @@
       <c r="B123" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="C123" s="0"/>
     </row>
     <row r="124" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
@@ -2099,6 +2147,7 @@
       <c r="B124" s="1" t="s">
         <v>146</v>
       </c>
+      <c r="C124" s="0"/>
     </row>
     <row r="125" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
@@ -2107,6 +2156,7 @@
       <c r="B125" s="1" t="s">
         <v>147</v>
       </c>
+      <c r="C125" s="0"/>
     </row>
     <row r="126" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="1" t="s">
@@ -2115,6 +2165,7 @@
       <c r="B126" s="1" t="s">
         <v>148</v>
       </c>
+      <c r="C126" s="0"/>
     </row>
     <row r="127" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
@@ -2123,6 +2174,7 @@
       <c r="B127" s="1" t="s">
         <v>149</v>
       </c>
+      <c r="C127" s="0"/>
     </row>
     <row r="128" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
@@ -2131,6 +2183,7 @@
       <c r="B128" s="1" t="s">
         <v>150</v>
       </c>
+      <c r="C128" s="0"/>
     </row>
     <row r="129" customFormat="false" ht="28.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="1" t="s">
@@ -2139,6 +2192,7 @@
       <c r="B129" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="C129" s="0"/>
     </row>
     <row r="130" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="1" t="s">
@@ -2147,6 +2201,7 @@
       <c r="B130" s="1" t="s">
         <v>152</v>
       </c>
+      <c r="C130" s="0"/>
     </row>
     <row r="131" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="1" t="s">
@@ -2155,6 +2210,7 @@
       <c r="B131" s="1" t="s">
         <v>153</v>
       </c>
+      <c r="C131" s="0"/>
     </row>
     <row r="132" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
@@ -2163,6 +2219,7 @@
       <c r="B132" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="C132" s="0"/>
     </row>
     <row r="133" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
@@ -2171,6 +2228,7 @@
       <c r="B133" s="1" t="s">
         <v>155</v>
       </c>
+      <c r="C133" s="0"/>
     </row>
     <row r="134" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
@@ -2179,6 +2237,7 @@
       <c r="B134" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="C134" s="0"/>
     </row>
     <row r="135" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
@@ -2187,6 +2246,7 @@
       <c r="B135" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="C135" s="0"/>
     </row>
     <row r="136" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
@@ -2989,6 +3049,70 @@
       </c>
       <c r="B217" s="2" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>